<commit_message>
change metrics & execute the experiment again
</commit_message>
<xml_diff>
--- a/experiment_2/queries.xlsx
+++ b/experiment_2/queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA/BA_Thesis/experiment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5B223F-4C19-6A40-BC55-45C38B0D49FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE3164F-2375-2C49-88C1-370C6A43B207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="820" windowWidth="28040" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
+    <workbookView xWindow="2200" yWindow="800" windowWidth="28040" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_1" sheetId="1" r:id="rId1"/>
@@ -60,30 +60,15 @@
     <t xml:space="preserve">Description </t>
   </si>
   <si>
-    <t>Name the building “Residential Building”</t>
-  </si>
-  <si>
     <t xml:space="preserve">Create </t>
   </si>
   <si>
     <t xml:space="preserve">Update </t>
   </si>
   <si>
-    <t>Change the name of the TestWall, to “Base Wall” and to its door to “Base Door”</t>
-  </si>
-  <si>
-    <t>Add a wall “Test Wall 1” and a “Test Door” in the building</t>
-  </si>
-  <si>
     <t>Create a room with “Test Wall 1”</t>
   </si>
   <si>
-    <t>Remove the door from the “Base Wall”</t>
-  </si>
-  <si>
-    <t>Delete all walls that creates with “Base Wall” a room</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delete </t>
   </si>
   <si>
@@ -115,6 +100,21 @@
   </si>
   <si>
     <t>MATCH (l:ifc__IfcLabel{express__hasString:["Base Wall"]})&lt;--(w1:ifc__IfcWall)&lt;-- (a1:ifc__IfcRelConnectsPathElements)--&gt;(w2:ifc__IfcWall)&lt;--(a2:ifc__IfcRelConnectsPathElements)--&gt; (w3:ifc__IfcWall)&lt;--(a3:ifc__IfcRelConnectsPathElements)--&gt;(w4:ifc__IfcWall)&lt;--(a4:ifc__IfcRelConnectsPathElements)--&gt;(w1) DETACH DELETE w1, w2, w3, w4, a1, a2, a3, a4</t>
+  </si>
+  <si>
+    <t>Add a wall "Test Wall 1" and a "Test Door" in the building</t>
+  </si>
+  <si>
+    <t>Name the building "Residential Building"</t>
+  </si>
+  <si>
+    <t>Change the name of the TestWall, to "Base Wall" and to its door to "Base Door"</t>
+  </si>
+  <si>
+    <t>Remove the door from the "Base Wall"</t>
+  </si>
+  <si>
+    <t>Delete all walls that creates with "Base Wall" a room</t>
   </si>
 </sst>
 </file>
@@ -173,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -319,7 +319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF80A08-7EAB-A54A-9D47-86295BB267AC}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,16 +508,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -525,16 +525,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -542,10 +542,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -559,16 +559,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -576,16 +576,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -593,16 +593,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Experiment 2] Changing some queries
</commit_message>
<xml_diff>
--- a/experiment_2/queries.xlsx
+++ b/experiment_2/queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA/BA_Thesis/experiment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE3164F-2375-2C49-88C1-370C6A43B207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86477BAF-0EAA-6D4B-B796-9098F48C96F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="800" windowWidth="28040" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_1" sheetId="1" r:id="rId1"/>
@@ -90,18 +90,6 @@
     <t>MATCH (l1:ifc__IfcLabel{express__hasString:["Test Door"]})&lt;--(d:ifc__IfcDoor)&lt;--(:ifc__IfcRelFillsElement)--&gt;(:ifc__IfcOpeningElement)&lt;--(:ifc__IfcRelVoidsElement)--&gt;(w:ifc__IfcWall)--&gt;(l2:ifc__IfcLabel{express__hasString:["Test Wall 1"]}) SET l2.express__hasString=["Base Wall"], l1.express__hasString=["Base Door"]</t>
   </si>
   <si>
-    <t>MATCH (w{Entity: "IfcWall", Name: "Base Wall"})--&gt;(o:IfcElement{Entity:"IfcOpeningElement"})--&gt;(d:IfcElement{Entity:"IfcDoor",Name:"Base Door"}) DETACH DELETE o,d</t>
-  </si>
-  <si>
-    <t>MATCH (:ifc__IfcLabel{express_hasString:["Basis Wall"]})&lt;--(:ifc__IfcWall)--&gt;(o:ifc__IfcOpeningElement)&lt;--(f:ifc__IfcRelFillsElement)--&gt;(d:ifc__IfcDoor)--&gt;(l:ifc__IfcLabel{express__hasString:["Base Door"]}) DETACH DELETE o,f,d,l</t>
-  </si>
-  <si>
-    <t>MATCH (w1{Entity: "IfcWall", Name: "Base Wall"})-[:IfcRelConnectsPathElements]-&gt;(w2:IfcElement{Entity:"IfcWall", Name:"Test Wall 2"})-[:IfcRelConnectsPathElements]-&gt;(w3:IfcElement{Entity:"IfcWall", Name:"Test Wall 3"})&lt;-[:IfcRelConnectsPathElements]-(w4:IfcElement{Entity:"IfcWall", Name:"Test Wall 4"})-[:IfcRelConnectsPathElements]-&gt;(w1) DETACH DELETE w1, w2, w3, w4</t>
-  </si>
-  <si>
-    <t>MATCH (l:ifc__IfcLabel{express__hasString:["Base Wall"]})&lt;--(w1:ifc__IfcWall)&lt;-- (a1:ifc__IfcRelConnectsPathElements)--&gt;(w2:ifc__IfcWall)&lt;--(a2:ifc__IfcRelConnectsPathElements)--&gt; (w3:ifc__IfcWall)&lt;--(a3:ifc__IfcRelConnectsPathElements)--&gt;(w4:ifc__IfcWall)&lt;--(a4:ifc__IfcRelConnectsPathElements)--&gt;(w1) DETACH DELETE w1, w2, w3, w4, a1, a2, a3, a4</t>
-  </si>
-  <si>
     <t>Add a wall "Test Wall 1" and a "Test Door" in the building</t>
   </si>
   <si>
@@ -115,6 +103,37 @@
   </si>
   <si>
     <t>Delete all walls that creates with "Base Wall" a room</t>
+  </si>
+  <si>
+    <t>MATCH  (w1:ifc__IfcWall)-[r1:ifc__name_IfcRoot]-&gt;(l1:ifc__IfcLabel{express__hasString:["Base Wall"]}),
+   (w2:ifc__IfcWall)-[r2:ifc__name_IfcRoot]-&gt;(l2:ifc__IfcLabel{express__hasString:["Test Wall 2"]}),
+       (w3:ifc__IfcWall)-[r3:ifc__name_IfcRoot]-&gt;(l3:ifc__IfcLabel{express__hasString:["Test Wall 3"]}),
+       (w4:ifc__IfcWall)-[r4:ifc__name_IfcRoot]-&gt;(l4:ifc__IfcLabel{express__hasString:["Test Wall 4"]}),
+       (w1)&lt;-[r5:ifc__relatingElement_IfcRelConnectsElements]- (n1:ifc__IfcRelConnectsPathElements)-[r6:ifc__relatedElement_IfcRelConnectsElements]-&gt;(w2) 
+	  &lt;-[r7:ifc__relatingElement_IfcRelConnectsElements]-(n2:ifc__IfcRelConnectsPathElements) -[r8:ifc__relatedElement_IfcRelConnectsElements]-&gt; (w3) 
+	 &lt;-[r9:ifc__relatingElement_IfcRelConnectsElements]-(n3:ifc__IfcRelConnectsPathElements)-[r10:ifc__relatedElement_IfcRelConnectsElements]-&gt;(w4) 
+             &lt;-[r11:ifc__relatedElement_IfcRelConnectsElements]-(n4:ifc__IfcRelConnectsPathElements)-[r12:ifc__relatingElement_IfcRelConnectsElements]-&gt;(w1)
+DETACH DELETE w1,w2,w3,w4,l1,l2,l3,l4,n1,n2,n3,n4,r1,r2,r3,r4,r5,r6,r7,r8,r9,r10,r11,r12</t>
+  </si>
+  <si>
+    <t>MATCH (:IfcElement{Entity:"IfcWall",Name:"Base Wall"})-[r1:IfcRelVoidsElement]-&gt;(o:IfcElement{Entity:"IfcOpeningElement"})-[r2:IfcRelFillsElement]-&gt;(d:IfcElement{Entity:"IfcDoor",Name:"Base Door"})
+DETACH DELETE o,d,r1,r2</t>
+  </si>
+  <si>
+    <t>MATCH (l:ifc__IfcLabel{express__hasString:["Base Door"]})&lt;-[r1:ifc__name_IfcRoot]-(n1:ifc__IfcDoor)
+				&lt;-[r2:ifc__relatedBuildingElement_IfcRelFillsElement]-(n2:ifc__IfcRelFillsElement)
+				-[r3:ifc__relatingOpeningElement_IfcRelFillsElement]-&gt;(n3:ifc__IfcOpeningElement)
+				&lt;-[r4:ifc__relatedOpeningElement_IfcRelVoidsElement]-(n4:ifc__IfcRelVoidsElement)
+				-[r5:ifc__relatingBuildingElement_IfcRelVoidsElement]-&gt;(:ifc__IfcWall)
+DETACH DELETE l,r1,r2,r3,r4,r5,n1,n2,n3,n4</t>
+  </si>
+  <si>
+    <t>MATCH (d {Entity:"IfcSite"})-[r1:IfcRelContainedInSpatialStructure]-&gt;(w1:IfcElement{Entity:"IfcWall",Name:"Base Wall"}),
+      (d)-[r2:IfcRelContainedInSpatialStructure]-&gt;(w2:IfcElement{Entity:"IfcWall",Name:"Test Wall 2"}),
+      (d)-[r3:IfcRelContainedInSpatialStructure]-&gt;(w3:IfcElement{Entity:"IfcWall",Name:"Test Wall 3"}),
+      (d)-[r4:IfcRelContainedInSpatialStructure]-&gt;(w4:IfcElement{Entity:"IfcWall",Name:"Test Wall 4"}),
+      (w1)-[r5:IfcRelConnectsPathElements]-&gt;(w2)-[r6:IfcRelConnectsPathElements]-&gt;(w3)&lt;-[r7:IfcRelConnectsPathElements]-(w4)-[r8:IfcRelConnectsPathElements]-&gt;(w1)
+DETACH DELETE w1,w2,w3,w4,r1,r2,r3,r4,r5,r6,r7,r8</t>
   </si>
 </sst>
 </file>
@@ -472,7 +491,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -542,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -559,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -571,38 +590,38 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Experiment 2] Change description column in the queries.xlsx
</commit_message>
<xml_diff>
--- a/experiment_2/queries.xlsx
+++ b/experiment_2/queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadine/Desktop/BA/BA_Thesis/experiment_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86477BAF-0EAA-6D4B-B796-9098F48C96F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B496CF-9B4E-2543-AFE0-36A36B5037F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{908B528D-F57B-5246-AF0C-CDF71ECB3D2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Type</t>
   </si>
@@ -134,6 +134,9 @@
       (d)-[r4:IfcRelContainedInSpatialStructure]-&gt;(w4:IfcElement{Entity:"IfcWall",Name:"Test Wall 4"}),
       (w1)-[r5:IfcRelConnectsPathElements]-&gt;(w2)-[r6:IfcRelConnectsPathElements]-&gt;(w3)&lt;-[r7:IfcRelConnectsPathElements]-(w4)-[r8:IfcRelConnectsPathElements]-&gt;(w1)
 DETACH DELETE w1,w2,w3,w4,r1,r2,r3,r4,r5,r6,r7,r8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -490,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF80A08-7EAB-A54A-9D47-86295BB267AC}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>